<commit_message>
update daily work plan
</commit_message>
<xml_diff>
--- a/doc/04.Schedule/开发计划.xlsx
+++ b/doc/04.Schedule/开发计划.xlsx
@@ -13,13 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="开发计划" sheetId="1" r:id="rId1"/>
-    <sheet name="前期准备计划" sheetId="3" r:id="rId2"/>
+    <sheet name="开发准备事项" sheetId="3" r:id="rId2"/>
     <sheet name="备份" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">开发计划!$A$2:$L$70</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">备份!$A$1:$L$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">前期准备计划!$A$1:$L$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">开发准备事项!$A$1:$L$12</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="298">
   <si>
     <t>编号</t>
   </si>
@@ -399,12 +399,6 @@
   </si>
   <si>
     <t>31</t>
-  </si>
-  <si>
-    <t>调整单</t>
-  </si>
-  <si>
-    <t>数据月结前对有误差的数据用调整单进行调整</t>
   </si>
   <si>
     <t>32</t>
@@ -980,9 +974,6 @@
 2、增加红股入帐和新股入帐交割单数据的买卖判断
 3、修改忽略数据导出excel文件的文件格式为xlsx</t>
     <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>81</t>
   </si>
   <si>
     <t>编制完成</t>
@@ -1113,16 +1104,7 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>账户的个股财务持仓/交割单持仓/当日委托持仓核对报表</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>账户收益核对功能</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、账户财务总收益/交割单总收益/当日委托总收益核对报表
-2、账户的个股财务收益/交割单收益/当日委托收益核对报表</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
@@ -1194,16 +1176,32 @@
     <t>70</t>
   </si>
   <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
     <t>1、调整单类别
 2、交割单收益与财务收益差额调整单的处理对象（交割单和当日委托数据调整，明确到交易账户）
 3、当日委托收益与交割单收益差额调整单的目标数据对象（当日委托数据调整，明确到交易员和交易账号）</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户起初数据管理功能</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>各账户每月期初数据：
+1、账户资金
+2、账户个股持仓</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>账户的个股财务持仓/交割单持仓/当日委托持仓核对报表</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、账户财务总收益/交割单总收益/当日委托总收益核对报表
+2、账户的个股财务收益/交割单收益/当日委托收益核对报表</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>81</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1488,15 +1486,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1806,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT95"/>
+  <dimension ref="A1:AT93"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1829,20 +1818,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="A1" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -1870,10 +1859,10 @@
         <v>7</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -1893,7 +1882,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>14</v>
@@ -2252,7 +2241,7 @@
     </row>
     <row r="13" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>11</v>
@@ -2396,7 +2385,7 @@
     </row>
     <row r="17" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>11</v>
@@ -2520,16 +2509,16 @@
         <v>13</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>105</v>
       </c>
       <c r="I20" s="24">
         <v>42664</v>
@@ -2558,16 +2547,16 @@
         <v>13</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I21" s="24">
         <v>42668</v>
@@ -2596,16 +2585,16 @@
         <v>13</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I22" s="24">
         <v>42670</v>
@@ -2622,7 +2611,7 @@
     </row>
     <row r="23" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>11</v>
@@ -2634,13 +2623,13 @@
         <v>13</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="24">
@@ -2670,13 +2659,13 @@
         <v>13</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="24">
@@ -2706,16 +2695,16 @@
         <v>13</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I25" s="24">
         <v>42677</v>
@@ -2744,13 +2733,13 @@
         <v>13</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="24">
@@ -2780,13 +2769,13 @@
         <v>13</v>
       </c>
       <c r="E27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="24">
@@ -2822,10 +2811,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I28" s="24">
         <v>42685</v>
@@ -2854,16 +2843,16 @@
         <v>13</v>
       </c>
       <c r="E29" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="H29" s="27" t="s">
         <v>147</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="H29" s="27" t="s">
-        <v>149</v>
       </c>
       <c r="I29" s="24">
         <v>42688</v>
@@ -2892,16 +2881,16 @@
         <v>13</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H30" s="27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I30" s="24">
         <v>42688</v>
@@ -2930,16 +2919,16 @@
         <v>13</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H31" s="27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I31" s="24">
         <v>42688</v>
@@ -2968,16 +2957,16 @@
         <v>13</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="I32" s="24">
         <v>42689</v>
@@ -3006,16 +2995,16 @@
         <v>13</v>
       </c>
       <c r="E33" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="H33" s="27" t="s">
-        <v>155</v>
       </c>
       <c r="I33" s="24">
         <v>42689</v>
@@ -3032,7 +3021,7 @@
     </row>
     <row r="34" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>11</v>
@@ -3044,16 +3033,16 @@
         <v>13</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>142</v>
       </c>
       <c r="I34" s="24">
         <v>42689</v>
@@ -3070,7 +3059,7 @@
     </row>
     <row r="35" spans="1:46" s="30" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>11</v>
@@ -3082,16 +3071,16 @@
         <v>13</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F35" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H35" s="27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I35" s="32">
         <v>42720</v>
@@ -3108,7 +3097,7 @@
     </row>
     <row r="36" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>11</v>
@@ -3120,16 +3109,16 @@
         <v>13</v>
       </c>
       <c r="E36" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="27" t="s">
         <v>172</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="H36" s="27" t="s">
-        <v>174</v>
       </c>
       <c r="I36" s="24">
         <v>42711</v>
@@ -3146,7 +3135,7 @@
     </row>
     <row r="37" spans="1:46" s="11" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>11</v>
@@ -3158,16 +3147,16 @@
         <v>13</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H37" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I37" s="24">
         <v>42712</v>
@@ -3184,7 +3173,7 @@
     </row>
     <row r="38" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>11</v>
@@ -3196,16 +3185,16 @@
         <v>13</v>
       </c>
       <c r="E38" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="H38" s="27" t="s">
         <v>169</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="H38" s="27" t="s">
-        <v>171</v>
       </c>
       <c r="I38" s="24">
         <v>42713</v>
@@ -3222,7 +3211,7 @@
     </row>
     <row r="39" spans="1:46" s="30" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B39" s="25" t="s">
         <v>11</v>
@@ -3234,16 +3223,16 @@
         <v>13</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H39" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I39" s="32">
         <v>42727</v>
@@ -3260,28 +3249,28 @@
     </row>
     <row r="40" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>103</v>
-      </c>
       <c r="F40" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H40" s="27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I40" s="32">
         <v>42731</v>
@@ -3298,7 +3287,7 @@
     </row>
     <row r="41" spans="1:46" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>11</v>
@@ -3310,13 +3299,13 @@
         <v>13</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="24">
@@ -3334,7 +3323,7 @@
     </row>
     <row r="42" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>11</v>
@@ -3346,16 +3335,16 @@
         <v>13</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I42" s="24">
         <v>42739</v>
@@ -3402,7 +3391,7 @@
     </row>
     <row r="43" spans="1:46" s="11" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>11</v>
@@ -3414,16 +3403,16 @@
         <v>13</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I43" s="24">
         <v>42740</v>
@@ -3468,9 +3457,9 @@
       <c r="AS43" s="16"/>
       <c r="AT43" s="16"/>
     </row>
-    <row r="44" spans="1:46" s="11" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:46" s="11" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>11</v>
@@ -3482,16 +3471,16 @@
         <v>13</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I44" s="24">
         <v>42741</v>
@@ -3536,9 +3525,9 @@
       <c r="AS44" s="16"/>
       <c r="AT44" s="16"/>
     </row>
-    <row r="45" spans="1:46" s="11" customFormat="1" ht="126.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:46" s="11" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>11</v>
@@ -3550,16 +3539,16 @@
         <v>13</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I45" s="24">
         <v>42741</v>
@@ -3606,7 +3595,7 @@
     </row>
     <row r="46" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>11</v>
@@ -3618,16 +3607,16 @@
         <v>13</v>
       </c>
       <c r="E46" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="I46" s="24">
         <v>42744</v>
@@ -3644,7 +3633,7 @@
     </row>
     <row r="47" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>11</v>
@@ -3656,16 +3645,16 @@
         <v>13</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I47" s="24">
         <v>42745</v>
@@ -3682,7 +3671,7 @@
     </row>
     <row r="48" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>11</v>
@@ -3694,16 +3683,16 @@
         <v>13</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I48" s="24">
         <v>42746</v>
@@ -3720,7 +3709,7 @@
     </row>
     <row r="49" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>11</v>
@@ -3732,16 +3721,16 @@
         <v>13</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I49" s="24">
         <v>42747</v>
@@ -3758,7 +3747,7 @@
     </row>
     <row r="50" spans="1:46" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>11</v>
@@ -3770,16 +3759,16 @@
         <v>13</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I50" s="24">
         <v>42748</v>
@@ -3796,7 +3785,7 @@
     </row>
     <row r="51" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>11</v>
@@ -3808,16 +3797,16 @@
         <v>13</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I51" s="24">
         <v>42751</v>
@@ -3836,7 +3825,7 @@
     </row>
     <row r="52" spans="1:46" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>11</v>
@@ -3848,16 +3837,16 @@
         <v>13</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I52" s="24">
         <v>42752</v>
@@ -3876,7 +3865,7 @@
     </row>
     <row r="53" spans="1:46" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>11</v>
@@ -3888,16 +3877,16 @@
         <v>13</v>
       </c>
       <c r="E53" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="I53" s="24">
         <v>42755</v>
@@ -3916,7 +3905,7 @@
     </row>
     <row r="54" spans="1:46" s="11" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>11</v>
@@ -3928,16 +3917,16 @@
         <v>13</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="H54" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="I54" s="24">
         <v>42755</v>
@@ -3956,7 +3945,7 @@
     </row>
     <row r="55" spans="1:46" s="11" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>11</v>
@@ -3968,16 +3957,16 @@
         <v>13</v>
       </c>
       <c r="E55" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="I55" s="24">
         <v>42773</v>
@@ -3989,14 +3978,14 @@
         <v>18</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
     </row>
     <row r="56" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>11</v>
@@ -4008,16 +3997,16 @@
         <v>13</v>
       </c>
       <c r="E56" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="I56" s="24">
         <v>42775</v>
@@ -4036,7 +4025,7 @@
     </row>
     <row r="57" spans="1:46" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>11</v>
@@ -4048,16 +4037,16 @@
         <v>13</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I57" s="24">
         <v>42775</v>
@@ -4069,14 +4058,14 @@
         <v>18</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
     </row>
-    <row r="58" spans="1:46" s="11" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:46" s="11" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>11</v>
@@ -4088,113 +4077,113 @@
         <v>13</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>244</v>
+        <v>145</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="G58" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="H58" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="I58" s="37">
-        <v>42780</v>
-      </c>
-      <c r="J58" s="37"/>
+        <v>15</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="I58" s="24">
+        <v>42781</v>
+      </c>
+      <c r="J58" s="24">
+        <v>42781</v>
+      </c>
       <c r="K58" s="9" t="s">
         <v>18</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>39</v>
+        <v>236</v>
       </c>
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
     </row>
-    <row r="59" spans="1:46" s="11" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="I59" s="24">
-        <v>42781</v>
-      </c>
-      <c r="J59" s="24">
-        <v>42781</v>
-      </c>
-      <c r="K59" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L59" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="M59" s="16"/>
-      <c r="N59" s="16"/>
-    </row>
-    <row r="60" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>162</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F59" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I59" s="32">
+        <v>42783</v>
+      </c>
+      <c r="J59" s="32">
+        <v>42787</v>
+      </c>
+      <c r="K59" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="L59" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="M59" s="29"/>
+      <c r="N59" s="29"/>
+    </row>
+    <row r="60" spans="1:46" s="11" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G60" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="H60" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="I60" s="32">
-        <v>42783</v>
-      </c>
-      <c r="J60" s="32">
-        <v>42788</v>
-      </c>
-      <c r="K60" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="L60" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="I60" s="24">
+        <v>42790</v>
+      </c>
+      <c r="J60" s="24">
+        <v>42790</v>
+      </c>
+      <c r="K60" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="M60" s="29"/>
-      <c r="N60" s="29"/>
     </row>
     <row r="61" spans="1:46" s="11" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>11</v>
@@ -4206,16 +4195,16 @@
         <v>13</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="I61" s="24">
         <v>42795</v>
@@ -4232,7 +4221,7 @@
     </row>
     <row r="62" spans="1:46" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>11</v>
@@ -4244,21 +4233,23 @@
         <v>13</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="I62" s="24">
         <v>42800</v>
       </c>
-      <c r="J62" s="24"/>
+      <c r="J62" s="24">
+        <v>42797</v>
+      </c>
       <c r="K62" s="9" t="s">
         <v>18</v>
       </c>
@@ -4298,7 +4289,7 @@
     </row>
     <row r="63" spans="1:46" s="11" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>11</v>
@@ -4310,16 +4301,16 @@
         <v>13</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="I63" s="8">
         <v>42804</v>
@@ -4364,7 +4355,7 @@
     </row>
     <row r="64" spans="1:46" s="11" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>11</v>
@@ -4376,16 +4367,16 @@
         <v>13</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I64" s="8">
         <v>42809</v>
@@ -4430,7 +4421,7 @@
     </row>
     <row r="65" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>11</v>
@@ -4442,16 +4433,16 @@
         <v>13</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="I65" s="8">
         <v>42814</v>
@@ -4496,7 +4487,7 @@
     </row>
     <row r="66" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>11</v>
@@ -4508,16 +4499,16 @@
         <v>13</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I66" s="8">
         <v>42822</v>
@@ -4532,7 +4523,7 @@
     </row>
     <row r="67" spans="1:46" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>11</v>
@@ -4544,16 +4535,16 @@
         <v>13</v>
       </c>
       <c r="E67" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="H67" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="I67" s="8">
         <v>42825</v>
@@ -4568,7 +4559,7 @@
     </row>
     <row r="68" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>11</v>
@@ -4580,16 +4571,16 @@
         <v>13</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I68" s="8"/>
       <c r="J68" s="21"/>
@@ -4602,7 +4593,7 @@
     </row>
     <row r="69" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>11</v>
@@ -4614,16 +4605,16 @@
         <v>13</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I69" s="8"/>
       <c r="J69" s="21"/>
@@ -4636,7 +4627,7 @@
     </row>
     <row r="70" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>11</v>
@@ -4648,16 +4639,16 @@
         <v>13</v>
       </c>
       <c r="E70" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G70" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F70" s="5" t="s">
+      <c r="H70" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="I70" s="8"/>
       <c r="J70" s="21"/>
@@ -4670,7 +4661,7 @@
     </row>
     <row r="71" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>11</v>
@@ -4704,7 +4695,7 @@
     </row>
     <row r="72" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>11</v>
@@ -4738,7 +4729,7 @@
     </row>
     <row r="73" spans="1:46" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>11</v>
@@ -4772,7 +4763,7 @@
     </row>
     <row r="74" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>11</v>
@@ -4804,7 +4795,7 @@
     </row>
     <row r="75" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>11</v>
@@ -4816,13 +4807,13 @@
         <v>13</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G75" s="7" t="s">
-        <v>83</v>
+      <c r="G75" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="8"/>
@@ -4836,7 +4827,7 @@
     </row>
     <row r="76" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>11</v>
@@ -4848,18 +4839,16 @@
         <v>13</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G76" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I76" s="8"/>
+      <c r="G76" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H76" s="6"/>
+      <c r="I76" s="23"/>
       <c r="J76" s="21"/>
       <c r="K76" s="9" t="s">
         <v>18</v>
@@ -4870,7 +4859,7 @@
     </row>
     <row r="77" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>11</v>
@@ -4882,13 +4871,13 @@
         <v>13</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G77" s="18" t="s">
-        <v>91</v>
+      <c r="G77" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="8"/>
@@ -4902,7 +4891,7 @@
     </row>
     <row r="78" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>11</v>
@@ -4914,16 +4903,16 @@
         <v>13</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G78" s="18" t="s">
-        <v>93</v>
+      <c r="G78" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="H78" s="6"/>
-      <c r="I78" s="23"/>
+      <c r="I78" s="21"/>
       <c r="J78" s="21"/>
       <c r="K78" s="9" t="s">
         <v>18</v>
@@ -4934,7 +4923,7 @@
     </row>
     <row r="79" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>11</v>
@@ -4951,8 +4940,8 @@
       <c r="F79" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G79" s="7" t="s">
-        <v>253</v>
+      <c r="G79" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="8"/>
@@ -4964,9 +4953,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>11</v>
@@ -4978,13 +4967,13 @@
         <v>13</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>96</v>
+        <v>21</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>97</v>
+        <v>289</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="21"/>
@@ -4996,9 +4985,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>11</v>
@@ -5015,11 +5004,11 @@
       <c r="F81" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G81" s="18" t="s">
-        <v>99</v>
+      <c r="G81" s="7" t="s">
+        <v>288</v>
       </c>
       <c r="H81" s="6"/>
-      <c r="I81" s="8"/>
+      <c r="I81" s="21"/>
       <c r="J81" s="21"/>
       <c r="K81" s="9" t="s">
         <v>18</v>
@@ -5028,9 +5017,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>11</v>
@@ -5042,13 +5031,13 @@
         <v>13</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="21"/>
@@ -5060,74 +5049,58 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:14" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H83" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="H83" s="6"/>
-      <c r="I83" s="21"/>
-      <c r="J83" s="21"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
       <c r="K83" s="9" t="s">
         <v>18</v>
       </c>
       <c r="L83" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>274</v>
-      </c>
+      <c r="M83" s="16"/>
+      <c r="N83" s="16"/>
+    </row>
+    <row r="84" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="7"/>
       <c r="H84" s="6"/>
       <c r="I84" s="21"/>
       <c r="J84" s="21"/>
-      <c r="K84" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L84" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="4" t="s">
-        <v>298</v>
-      </c>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+    </row>
+    <row r="85" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="4"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="20"/>
@@ -5140,7 +5113,7 @@
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
     </row>
-    <row r="86" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -5154,7 +5127,7 @@
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
     </row>
-    <row r="87" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -5168,7 +5141,7 @@
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
     </row>
-    <row r="88" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -5182,7 +5155,7 @@
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
     </row>
-    <row r="89" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -5196,7 +5169,7 @@
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -5210,7 +5183,7 @@
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
     </row>
-    <row r="91" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -5224,7 +5197,7 @@
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
     </row>
-    <row r="92" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -5238,7 +5211,7 @@
       <c r="K92" s="9"/>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -5251,34 +5224,6 @@
       <c r="J93" s="21"/>
       <c r="K93" s="9"/>
       <c r="L93" s="9"/>
-    </row>
-    <row r="94" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="4"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="7"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="21"/>
-      <c r="J94" s="21"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
-    </row>
-    <row r="95" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="4"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="7"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="21"/>
-      <c r="J95" s="21"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:L38"/>
@@ -5322,20 +5267,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="A1" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -5363,10 +5308,10 @@
         <v>7</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -5386,19 +5331,19 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -5419,16 +5364,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>266</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -5449,16 +5394,16 @@
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -5479,16 +5424,16 @@
         <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
@@ -5509,16 +5454,16 @@
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -5539,16 +5484,16 @@
         <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -5569,16 +5514,16 @@
         <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5599,7 +5544,7 @@
         <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="7"/>
@@ -5623,7 +5568,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="7"/>
@@ -5647,7 +5592,7 @@
         <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="7"/>
@@ -5685,20 +5630,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="A1" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -5726,10 +5671,10 @@
         <v>7</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -5740,7 +5685,7 @@
     </row>
     <row r="3" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
@@ -5772,7 +5717,7 @@
     </row>
     <row r="4" spans="1:12" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -5804,7 +5749,7 @@
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Modify Entity and Map
</commit_message>
<xml_diff>
--- a/doc/04.Schedule/开发计划.xlsx
+++ b/doc/04.Schedule/开发计划.xlsx
@@ -1182,10 +1182,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>账户起初数据管理功能</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>各账户每月期初数据：
 1、账户资金
 2、账户个股持仓</t>
@@ -1202,6 +1198,10 @@
   </si>
   <si>
     <t>81</t>
+  </si>
+  <si>
+    <t>账户期初数据管理功能</t>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1797,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT93"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A52" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="M61" sqref="M61"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4163,10 +4163,10 @@
         <v>15</v>
       </c>
       <c r="G60" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="H60" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="I60" s="24">
         <v>42790</v>
@@ -4204,7 +4204,7 @@
         <v>273</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I61" s="24">
         <v>42795</v>
@@ -4242,7 +4242,7 @@
         <v>274</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I62" s="24">
         <v>42800</v>
@@ -4287,9 +4287,9 @@
       <c r="AS62" s="16"/>
       <c r="AT62" s="16"/>
     </row>
-    <row r="63" spans="1:46" s="11" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:46" s="11" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>11</v>
@@ -4301,21 +4301,23 @@
         <v>13</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="I63" s="8">
+        <v>278</v>
+      </c>
+      <c r="I63" s="24">
         <v>42804</v>
       </c>
-      <c r="J63" s="8"/>
+      <c r="J63" s="24">
+        <v>42804</v>
+      </c>
       <c r="K63" s="9" t="s">
         <v>18</v>
       </c>
@@ -4353,9 +4355,9 @@
       <c r="AS63" s="16"/>
       <c r="AT63" s="16"/>
     </row>
-    <row r="64" spans="1:46" s="11" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>11</v>
@@ -4367,19 +4369,19 @@
         <v>13</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I64" s="8">
-        <v>42809</v>
+        <v>42811</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="9" t="s">
@@ -4419,9 +4421,9 @@
       <c r="AS64" s="16"/>
       <c r="AT64" s="16"/>
     </row>
-    <row r="65" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:46" s="11" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>11</v>
@@ -4433,19 +4435,19 @@
         <v>13</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="I65" s="8">
-        <v>42814</v>
+        <v>42818</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="9" t="s">
@@ -5051,7 +5053,7 @@
     </row>
     <row r="83" spans="1:14" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add investor risk control
</commit_message>
<xml_diff>
--- a/doc/04.Schedule/开发计划.xlsx
+++ b/doc/04.Schedule/开发计划.xlsx
@@ -17,7 +17,7 @@
     <sheet name="备份" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">开发计划!$A$2:$L$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">开发计划!$A$2:$L$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">备份!$A$1:$L$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">开发准备事项!$A$1:$L$12</definedName>
   </definedNames>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="301">
   <si>
     <t>编号</t>
   </si>
@@ -1203,12 +1203,24 @@
     <t>账户期初数据管理功能</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
+  <si>
+    <t>分析决策表</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人首页</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>投资人员风控信息</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1797,11 +1809,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT93"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A64" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="5.5" style="13" customWidth="1"/>
     <col min="2" max="3" width="9.25" style="14" customWidth="1"/>
@@ -1817,7 +1829,7 @@
     <col min="13" max="16384" width="10" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1">
       <c r="A1" s="35" t="s">
         <v>188</v>
       </c>
@@ -1833,7 +1845,7 @@
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
     </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1871,7 +1883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="25.15" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1909,7 +1921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="25.15" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="25.15" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1983,7 +1995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="25.15" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="25.15" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
@@ -2057,7 +2069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="25.15" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -2093,7 +2105,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -2131,7 +2143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="25.15" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -2167,7 +2179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="25.15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -2203,7 +2215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="25.15" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -2239,7 +2251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="25.15" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>154</v>
       </c>
@@ -2275,7 +2287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="25.15" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="25.15" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -2347,7 +2359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="27.75" customHeight="1">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
@@ -2383,7 +2395,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="25.15" customHeight="1">
       <c r="A17" s="4" t="s">
         <v>155</v>
       </c>
@@ -2421,7 +2433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="25.15" customHeight="1">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
@@ -2457,7 +2469,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="25.15" customHeight="1">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
@@ -2495,7 +2507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="25.15" customHeight="1">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" ht="25.15" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
@@ -2571,7 +2583,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>61</v>
       </c>
@@ -2609,7 +2621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>156</v>
       </c>
@@ -2645,7 +2657,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -2681,7 +2693,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>64</v>
       </c>
@@ -2719,7 +2731,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -2755,7 +2767,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>72</v>
       </c>
@@ -2791,7 +2803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A28" s="4" t="s">
         <v>76</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A29" s="4" t="s">
         <v>79</v>
       </c>
@@ -2867,7 +2879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="11" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="11" customFormat="1" ht="26.25" customHeight="1">
       <c r="A30" s="4" t="s">
         <v>82</v>
       </c>
@@ -2905,7 +2917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="11" customFormat="1" ht="33" customHeight="1">
       <c r="A31" s="4" t="s">
         <v>84</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A32" s="4" t="s">
         <v>85</v>
       </c>
@@ -2981,7 +2993,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A33" s="4" t="s">
         <v>86</v>
       </c>
@@ -3019,7 +3031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A34" s="4" t="s">
         <v>87</v>
       </c>
@@ -3057,7 +3069,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:46" s="30" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:46" s="30" customFormat="1" ht="42.75" customHeight="1">
       <c r="A35" s="4" t="s">
         <v>90</v>
       </c>
@@ -3095,7 +3107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>92</v>
       </c>
@@ -3133,7 +3145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:46" s="11" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:46" s="11" customFormat="1" ht="32.25" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>93</v>
       </c>
@@ -3171,7 +3183,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>96</v>
       </c>
@@ -3209,7 +3221,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:46" s="30" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:46" s="30" customFormat="1" ht="54" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>98</v>
       </c>
@@ -3247,7 +3259,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>99</v>
       </c>
@@ -3285,7 +3297,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:46" s="11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:46" s="11" customFormat="1" ht="23.25" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>100</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>104</v>
       </c>
@@ -3389,7 +3401,7 @@
       <c r="AS42" s="16"/>
       <c r="AT42" s="16"/>
     </row>
-    <row r="43" spans="1:46" s="11" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:46" s="11" customFormat="1" ht="82.5" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>107</v>
       </c>
@@ -3457,7 +3469,7 @@
       <c r="AS43" s="16"/>
       <c r="AT43" s="16"/>
     </row>
-    <row r="44" spans="1:46" s="11" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:46" s="11" customFormat="1" ht="57.75" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>109</v>
       </c>
@@ -3525,7 +3537,7 @@
       <c r="AS44" s="16"/>
       <c r="AT44" s="16"/>
     </row>
-    <row r="45" spans="1:46" s="11" customFormat="1" ht="108.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:46" s="11" customFormat="1" ht="108.75" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>111</v>
       </c>
@@ -3593,7 +3605,7 @@
       <c r="AS45" s="16"/>
       <c r="AT45" s="16"/>
     </row>
-    <row r="46" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>113</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>116</v>
       </c>
@@ -3669,7 +3681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:46" s="11" customFormat="1" ht="49.5" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>117</v>
       </c>
@@ -3707,7 +3719,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>120</v>
       </c>
@@ -3745,7 +3757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:46" s="11" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:46" s="11" customFormat="1" ht="60" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>124</v>
       </c>
@@ -3783,7 +3795,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:46" s="11" customFormat="1" ht="38.25" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>127</v>
       </c>
@@ -3823,7 +3835,7 @@
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
     </row>
-    <row r="52" spans="1:46" s="11" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:46" s="11" customFormat="1" ht="19.5" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>129</v>
       </c>
@@ -3863,7 +3875,7 @@
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
     </row>
-    <row r="53" spans="1:46" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:46" s="11" customFormat="1" ht="22.5" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>132</v>
       </c>
@@ -3903,7 +3915,7 @@
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
     </row>
-    <row r="54" spans="1:46" s="11" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:46" s="11" customFormat="1" ht="35.25" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>137</v>
       </c>
@@ -3943,7 +3955,7 @@
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
     </row>
-    <row r="55" spans="1:46" s="11" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:46" s="11" customFormat="1" ht="59.25" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>144</v>
       </c>
@@ -3983,7 +3995,7 @@
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
     </row>
-    <row r="56" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>150</v>
       </c>
@@ -4023,7 +4035,7 @@
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
     </row>
-    <row r="57" spans="1:46" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:46" s="11" customFormat="1" ht="33" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>160</v>
       </c>
@@ -4063,7 +4075,7 @@
       <c r="M57" s="16"/>
       <c r="N57" s="16"/>
     </row>
-    <row r="58" spans="1:46" s="11" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:46" s="11" customFormat="1" ht="75.75" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>161</v>
       </c>
@@ -4103,7 +4115,7 @@
       <c r="M58" s="16"/>
       <c r="N58" s="16"/>
     </row>
-    <row r="59" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:46" s="30" customFormat="1" ht="38.25" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>162</v>
       </c>
@@ -4143,7 +4155,7 @@
       <c r="M59" s="29"/>
       <c r="N59" s="29"/>
     </row>
-    <row r="60" spans="1:46" s="11" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:46" s="11" customFormat="1" ht="53.25" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>163</v>
       </c>
@@ -4181,7 +4193,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:46" s="11" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:46" s="11" customFormat="1" ht="39.75" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>189</v>
       </c>
@@ -4219,7 +4231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:46" s="11" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:46" s="11" customFormat="1" ht="57" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>190</v>
       </c>
@@ -4287,7 +4299,7 @@
       <c r="AS62" s="16"/>
       <c r="AT62" s="16"/>
     </row>
-    <row r="63" spans="1:46" s="11" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:46" s="11" customFormat="1" ht="42.75" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>192</v>
       </c>
@@ -4355,7 +4367,7 @@
       <c r="AS63" s="16"/>
       <c r="AT63" s="16"/>
     </row>
-    <row r="64" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:46" s="11" customFormat="1" ht="43.5" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>193</v>
       </c>
@@ -4421,7 +4433,7 @@
       <c r="AS64" s="16"/>
       <c r="AT64" s="16"/>
     </row>
-    <row r="65" spans="1:46" s="11" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:46" s="11" customFormat="1" ht="100.5" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>191</v>
       </c>
@@ -4487,7 +4499,7 @@
       <c r="AS65" s="16"/>
       <c r="AT65" s="16"/>
     </row>
-    <row r="66" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:46" s="11" customFormat="1" ht="25.5" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>194</v>
       </c>
@@ -4523,7 +4535,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:46" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:46" s="11" customFormat="1" ht="28.5" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>195</v>
       </c>
@@ -4559,134 +4571,80 @@
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H68" s="6"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+    </row>
+    <row r="69" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="H69" s="6"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+    </row>
+    <row r="70" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="H70" s="6"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+    </row>
+    <row r="71" spans="1:46" ht="25.15" customHeight="1">
+      <c r="A71" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" s="5" t="s">
+      <c r="B71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F68" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G68" s="6" t="s">
+      <c r="F71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H68" s="6" t="s">
+      <c r="H71" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I68" s="8"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L68" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I69" s="8"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L69" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I70" s="8"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L70" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G71" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I71" s="21"/>
+      <c r="I71" s="8"/>
       <c r="J71" s="21"/>
       <c r="K71" s="9" t="s">
         <v>18</v>
@@ -4695,9 +4653,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:46" ht="25.15" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>291</v>
+        <v>197</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>11</v>
@@ -4709,19 +4667,19 @@
         <v>13</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G72" s="18" t="s">
-        <v>74</v>
+      <c r="G72" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
+        <v>128</v>
+      </c>
+      <c r="I72" s="8"/>
+      <c r="J72" s="21"/>
       <c r="K72" s="9" t="s">
         <v>18</v>
       </c>
@@ -4729,9 +4687,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:46" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>11</v>
@@ -4743,19 +4701,19 @@
         <v>13</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G73" s="18" t="s">
-        <v>77</v>
+        <v>134</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I73" s="22"/>
-      <c r="J73" s="22"/>
+        <v>136</v>
+      </c>
+      <c r="I73" s="8"/>
+      <c r="J73" s="21"/>
       <c r="K73" s="9" t="s">
         <v>18</v>
       </c>
@@ -4763,9 +4721,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:46" ht="25.15" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>200</v>
+        <v>290</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>11</v>
@@ -4777,15 +4735,17 @@
         <v>13</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G74" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="H74" s="6"/>
+      <c r="G74" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="I74" s="21"/>
       <c r="J74" s="21"/>
       <c r="K74" s="9" t="s">
@@ -4795,9 +4755,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:46" ht="25.15" customHeight="1">
       <c r="A75" s="4" t="s">
-        <v>201</v>
+        <v>291</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>11</v>
@@ -4809,17 +4769,19 @@
         <v>13</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="H75" s="6"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="21"/>
+        <v>74</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
       <c r="K75" s="9" t="s">
         <v>18</v>
       </c>
@@ -4827,9 +4789,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:46" ht="29.25" customHeight="1">
       <c r="A76" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>11</v>
@@ -4841,17 +4803,19 @@
         <v>13</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="H76" s="6"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
       <c r="K76" s="9" t="s">
         <v>18</v>
       </c>
@@ -4859,9 +4823,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:46" ht="25.15" customHeight="1">
       <c r="A77" s="4" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>11</v>
@@ -4873,16 +4837,16 @@
         <v>13</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G77" s="7" t="s">
-        <v>250</v>
+      <c r="G77" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="H77" s="6"/>
-      <c r="I77" s="8"/>
+      <c r="I77" s="21"/>
       <c r="J77" s="21"/>
       <c r="K77" s="9" t="s">
         <v>18</v>
@@ -4891,9 +4855,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:46" ht="25.15" customHeight="1">
       <c r="A78" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>11</v>
@@ -4905,16 +4869,16 @@
         <v>13</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G78" s="7" t="s">
-        <v>95</v>
+      <c r="G78" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="H78" s="6"/>
-      <c r="I78" s="21"/>
+      <c r="I78" s="8"/>
       <c r="J78" s="21"/>
       <c r="K78" s="9" t="s">
         <v>18</v>
@@ -4923,9 +4887,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:46" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:46" ht="25.15" customHeight="1">
       <c r="A79" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>11</v>
@@ -4937,16 +4901,16 @@
         <v>13</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G79" s="18" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H79" s="6"/>
-      <c r="I79" s="8"/>
+      <c r="I79" s="23"/>
       <c r="J79" s="21"/>
       <c r="K79" s="9" t="s">
         <v>18</v>
@@ -4955,9 +4919,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:46" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:46" ht="25.15" customHeight="1">
       <c r="A80" s="4" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>11</v>
@@ -4975,10 +4939,10 @@
         <v>15</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>289</v>
+        <v>250</v>
       </c>
       <c r="H80" s="6"/>
-      <c r="I80" s="21"/>
+      <c r="I80" s="8"/>
       <c r="J80" s="21"/>
       <c r="K80" s="9" t="s">
         <v>18</v>
@@ -4987,9 +4951,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:14" ht="25.15" customHeight="1">
       <c r="A81" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>11</v>
@@ -5001,13 +4965,13 @@
         <v>13</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>288</v>
+        <v>95</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="21"/>
@@ -5019,9 +4983,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:14" ht="25.15" customHeight="1">
       <c r="A82" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>11</v>
@@ -5033,16 +4997,16 @@
         <v>13</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>145</v>
+        <v>21</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G82" s="7" t="s">
-        <v>271</v>
+      <c r="G82" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="H82" s="6"/>
-      <c r="I82" s="21"/>
+      <c r="I82" s="8"/>
       <c r="J82" s="21"/>
       <c r="K82" s="9" t="s">
         <v>18</v>
@@ -5051,9 +5015,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:14" s="11" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A83" s="4" t="s">
-        <v>296</v>
+        <v>205</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>11</v>
@@ -5065,71 +5029,125 @@
         <v>13</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>242</v>
+        <v>21</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
+        <v>289</v>
+      </c>
+      <c r="H83" s="6"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
       <c r="K83" s="9" t="s">
         <v>18</v>
       </c>
       <c r="L83" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="M83" s="16"/>
-      <c r="N83" s="16"/>
-    </row>
-    <row r="84" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="4"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="7"/>
+    </row>
+    <row r="84" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
+      <c r="A84" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>288</v>
+      </c>
       <c r="H84" s="6"/>
       <c r="I84" s="21"/>
       <c r="J84" s="21"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-    </row>
-    <row r="85" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="4"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="7"/>
+      <c r="K84" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L84" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
+      <c r="A85" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>271</v>
+      </c>
       <c r="H85" s="6"/>
       <c r="I85" s="21"/>
       <c r="J85" s="21"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-    </row>
-    <row r="86" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="4"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="21"/>
-      <c r="J86" s="21"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
-    </row>
-    <row r="87" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K85" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L85" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" s="11" customFormat="1" ht="39" customHeight="1">
+      <c r="A86" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L86" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M86" s="16"/>
+      <c r="N86" s="16"/>
+    </row>
+    <row r="87" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
@@ -5143,7 +5161,7 @@
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
     </row>
-    <row r="88" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -5157,7 +5175,7 @@
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
     </row>
-    <row r="89" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -5171,7 +5189,7 @@
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
     </row>
-    <row r="90" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -5185,7 +5203,7 @@
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
     </row>
-    <row r="91" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -5199,7 +5217,7 @@
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
     </row>
-    <row r="92" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -5213,7 +5231,7 @@
       <c r="K92" s="9"/>
       <c r="L92" s="9"/>
     </row>
-    <row r="93" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:14" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
@@ -5255,7 +5273,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="5.875" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
@@ -5268,7 +5286,7 @@
     <col min="12" max="12" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1">
       <c r="A1" s="35" t="s">
         <v>188</v>
       </c>
@@ -5284,7 +5302,7 @@
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
     </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5322,7 +5340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="16" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" s="16" customFormat="1" ht="37.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -5352,7 +5370,7 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" s="16" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="81" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -5382,7 +5400,7 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" s="16" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" s="16" customFormat="1" ht="73.5" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -5412,7 +5430,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:12" s="16" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" s="16" customFormat="1" ht="123" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -5442,7 +5460,7 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" s="16" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" s="16" customFormat="1" ht="53.25" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
@@ -5472,7 +5490,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" s="11" customFormat="1" ht="25.15" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -5502,7 +5520,7 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" s="16" customFormat="1" ht="41.25" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -5532,7 +5550,7 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -5556,7 +5574,7 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
@@ -5580,7 +5598,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
@@ -5623,7 +5641,7 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="4" max="4" width="14.25" customWidth="1"/>
@@ -5631,7 +5649,7 @@
     <col min="8" max="8" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="25.15" customHeight="1">
       <c r="A1" s="35" t="s">
         <v>188</v>
       </c>
@@ -5647,7 +5665,7 @@
       <c r="K1" s="35"/>
       <c r="L1" s="35"/>
     </row>
-    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="10" customFormat="1" ht="25.15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5685,7 +5703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>251</v>
       </c>
@@ -5717,7 +5735,7 @@
       </c>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="29.25" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>252</v>
       </c>
@@ -5749,7 +5767,7 @@
       </c>
       <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" s="16" customFormat="1" ht="25.15" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>253</v>
       </c>

</xml_diff>